<commit_message>
Data and protocol update
</commit_message>
<xml_diff>
--- a/Samples 1.xlsx
+++ b/Samples 1.xlsx
@@ -34,9 +34,6 @@
     <t>∆m (g)</t>
   </si>
   <si>
-    <t>Total NH4 Mass (g)</t>
-  </si>
-  <si>
     <t>Salt Type</t>
   </si>
   <si>
@@ -47,6 +44,9 @@
   </si>
   <si>
     <t>Percent Yield @ 30 min.</t>
+  </si>
+  <si>
+    <t>Total NH3 Mass (g)</t>
   </si>
 </sst>
 </file>
@@ -101,8 +101,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -115,15 +121,21 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -191,10 +203,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.568</c:v>
+                  <c:v>0.53625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.301308</c:v>
+                  <c:v>0.284481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -206,10 +218,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>57.74647887323995</c:v>
+                  <c:v>61.16550116550171</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.30780463843988</c:v>
+                  <c:v>87.17629648376884</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -256,10 +268,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.703</c:v>
+                  <c:v>0.66375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41593</c:v>
+                  <c:v>0.3926975</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -271,10 +283,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>52.34708392603058</c:v>
+                  <c:v>55.44256120527231</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59.8658428100905</c:v>
+                  <c:v>63.40758471851983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -289,11 +301,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2114031240"/>
-        <c:axId val="2114036952"/>
+        <c:axId val="2132613928"/>
+        <c:axId val="2132606200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2114031240"/>
+        <c:axId val="2132613928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -303,12 +315,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114036952"/>
+        <c:crossAx val="2132606200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2114036952"/>
+        <c:axId val="2132606200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -319,14 +331,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114031240"/>
+        <c:crossAx val="2132613928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -699,7 +710,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -727,13 +738,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -752,15 +763,15 @@
         <v>0.32800000000000296</v>
       </c>
       <c r="E2">
-        <f>0.127+0.441</f>
-        <v>0.56800000000000006</v>
+        <f>0.75*0.127+0.441</f>
+        <v>0.53625</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <f>100*D2/E2</f>
-        <v>57.746478873239951</v>
+        <v>61.165501165501716</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -778,15 +789,15 @@
         <v>0.24799999999999045</v>
       </c>
       <c r="E3">
-        <f>0.067308+0.234</f>
-        <v>0.30130800000000002</v>
+        <f>0.75*0.067308+0.234</f>
+        <v>0.28448100000000004</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <f>100*D3/E3</f>
-        <v>82.307804638439876</v>
+        <v>87.176296483768837</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -804,15 +815,15 @@
         <v>0.367999999999995</v>
       </c>
       <c r="E4">
-        <f>0.157+0.546</f>
-        <v>0.70300000000000007</v>
+        <f>0.75*0.157+0.546</f>
+        <v>0.66375000000000006</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4">
         <f>100*D4/E4</f>
-        <v>52.347083926030578</v>
+        <v>55.442561205272312</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -830,15 +841,15 @@
         <v>0.24900000000000944</v>
       </c>
       <c r="E5">
-        <f>0.09293+0.323</f>
-        <v>0.41593000000000002</v>
+        <f>0.75*0.09293+0.323</f>
+        <v>0.39269750000000003</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5">
         <f>100*D5/E5</f>
-        <v>59.865842810090498</v>
+        <v>63.407584718519828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>